<commit_message>
Bugfix: Added No in 2 excel templates
</commit_message>
<xml_diff>
--- a/bin/constants/ResultListTemplate.xlsx
+++ b/bin/constants/ResultListTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA667F3-1FC8-4D87-BD35-D626DFAC5B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE09064-E54A-4F26-80B6-3AF4ED137EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Car Maker</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>AISIN Sub-Premium/AM</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,11 +162,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -178,6 +207,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -460,94 +495,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="7.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10" style="1" customWidth="1"/>
     <col min="16" max="17" width="15.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="1" customWidth="1"/>
     <col min="19" max="20" width="15.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="1"/>
+    <col min="21" max="22" width="14.28515625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+    <row r="2" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -560,45 +597,47 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:U2"/>
+  <mergeCells count="18">
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bugfix: Removing a few logs, fixing Download template, fixing Download Partlist where competiter not found
</commit_message>
<xml_diff>
--- a/bin/constants/ResultListTemplate.xlsx
+++ b/bin/constants/ResultListTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE09064-E54A-4F26-80B6-3AF4ED137EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC63619C-D988-414F-9E51-E0C7C0912DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,11 @@
     <col min="12" max="13" width="12.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="7.140625" style="3" customWidth="1"/>
     <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="17" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="1" customWidth="1"/>
-    <col min="19" max="20" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="1" customWidth="1"/>
     <col min="21" max="22" width="14.28515625" style="1" customWidth="1"/>
     <col min="23" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -620,11 +622,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -638,6 +635,11 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>